<commit_message>
BnB algorithm is ready!
</commit_message>
<xml_diff>
--- a/lab4/lab4.xlsx
+++ b/lab4/lab4.xlsx
@@ -1,16 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37EBC34-7FA7-44F1-8014-AB6679B26E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBFBFA9-35F5-40A0-9E90-F836ED66DF3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commisvoyageur Algorithms" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -27,10 +36,6 @@
   <si>
     <t>Время
 фактическое</t>
-  </si>
-  <si>
-    <t>Параметры:
-Размер массива:</t>
   </si>
   <si>
     <t>Операций в секунду</t>
@@ -51,8 +56,12 @@
     <t>Локальный поиск с выбором</t>
   </si>
   <si>
+    <t>Параметры:
+Кол-во вершин:</t>
+  </si>
+  <si>
     <t xml:space="preserve">
-Размер массива:</t>
+Кол-во вершин:</t>
   </si>
 </sst>
 </file>
@@ -79,7 +88,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -167,6 +176,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -183,16 +205,10 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -202,9 +218,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -213,6 +226,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -222,10 +239,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1250,6 +1272,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1259,6 +1311,36 @@
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>6.7347400000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99594400000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5724200000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.783300000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>52.574300000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>118.78400000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>212.196</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>384.61799999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>732.68100000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1455.61</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1314,6 +1396,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1591,12 +1703,12 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Commisvoyageur Algorithms'!$L$2</c:f>
+              <c:f>'Commisvoyageur Algorithms'!$O$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>Время
-фактическое</c:v>
+аналитическое</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1636,10 +1748,40 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Commisvoyageur Algorithms'!$L$3:$L$12</c:f>
+              <c:f>'Commisvoyageur Algorithms'!$O$3:$O$12</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1655,12 +1797,12 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Commisvoyageur Algorithms'!$K$2</c:f>
+              <c:f>'Commisvoyageur Algorithms'!$P$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>Время
-аналитическое</c:v>
+фактическое</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1700,7 +1842,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Commisvoyageur Algorithms'!$K$3:$K$12</c:f>
+              <c:f>'Commisvoyageur Algorithms'!$P$3:$P$12</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4594,105 +4736,105 @@
   <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="23"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="23"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="22"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="22"/>
-      <c r="P1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="24"/>
       <c r="R1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>3</v>
+      <c r="A2" s="25" t="s">
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="25" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="26" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="25" t="s">
         <v>10</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="26" t="s">
         <v>1</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="27" t="s">
         <v>10</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="O2" s="15" t="s">
+      <c r="O2" s="13" t="s">
         <v>1</v>
       </c>
       <c r="P2" s="3" t="s">
@@ -4703,425 +4845,495 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>4</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="19">
         <v>667</v>
       </c>
-      <c r="C3" s="9">
-        <f t="shared" ref="C3:C12" si="0">B3/$R$2</f>
+      <c r="C3" s="6">
+        <f t="shared" ref="C3:C11" si="0">B3/$R$2</f>
         <v>3.2696078431372549E-7</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="10">
         <v>0</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>1000</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="19">
         <v>25543038</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="6">
         <f t="shared" ref="G3:G12" si="1">F3/$R$2</f>
         <v>1.252109705882353E-2</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="12">
         <v>1.9010099999999999E-2</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="9">
+      <c r="I3" s="5">
+        <v>100</v>
+      </c>
+      <c r="J3" s="19"/>
+      <c r="K3" s="6">
         <f t="shared" ref="K3:K11" si="2">J3/$R$2</f>
         <v>0</v>
       </c>
-      <c r="L3" s="12"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="9">
-        <f t="shared" ref="O3:O11" si="3">N3/$R$2</f>
+      <c r="L3" s="10">
+        <v>6.7347400000000002E-2</v>
+      </c>
+      <c r="M3" s="5"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="8">
+        <f t="shared" ref="O3:P11" si="3">N3/$R$2</f>
         <v>0</v>
       </c>
-      <c r="P3" s="12"/>
-      <c r="R3" s="18"/>
+      <c r="P3" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R3" s="15"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>5</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="19">
         <v>3250</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <f t="shared" si="0"/>
         <v>1.5931372549019608E-6</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="10">
         <v>0</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>2000</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="19">
         <v>102087548</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <f t="shared" si="1"/>
         <v>5.004291568627451E-2</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="12">
         <v>5.5119399999999999E-2</v>
       </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="7">
+      <c r="I4" s="5">
+        <v>200</v>
+      </c>
+      <c r="J4" s="19"/>
+      <c r="K4" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L4" s="12"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="7">
+      <c r="L4" s="10">
+        <v>0.99594400000000005</v>
+      </c>
+      <c r="M4" s="5"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P4" s="12"/>
+      <c r="P4" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>6</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="19">
         <v>20257</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <f t="shared" si="0"/>
         <v>9.9299019607843143E-6</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="10">
         <v>0</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>3000</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="19">
         <v>229631988</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <f t="shared" si="1"/>
         <v>0.1125647</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="12">
         <v>0.140627</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="7">
+      <c r="I5" s="5">
+        <v>300</v>
+      </c>
+      <c r="J5" s="19"/>
+      <c r="K5" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L5" s="12"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="7">
+      <c r="L5" s="10">
+        <v>5.5724200000000002</v>
+      </c>
+      <c r="M5" s="5"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P5" s="12"/>
+      <c r="P5" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>7</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="19">
         <v>149872</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <f t="shared" si="0"/>
         <v>7.3466666666666673E-5</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="10">
         <v>0</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>5000</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="19">
         <v>637721678</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <f t="shared" si="1"/>
         <v>0.31260866568627449</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="12">
         <v>0.41103499999999998</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="7">
+      <c r="I6" s="5">
+        <v>400</v>
+      </c>
+      <c r="J6" s="21"/>
+      <c r="K6" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L6" s="12"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="7">
+      <c r="L6" s="10">
+        <v>18.783300000000001</v>
+      </c>
+      <c r="M6" s="5"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P6" s="12"/>
+      <c r="P6" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>8</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="19">
         <v>1270207</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <f t="shared" si="0"/>
         <v>6.2265049019607848E-4</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="10">
         <v>1.0212999999999999E-3</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>10000</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="19">
         <v>2550441978</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <f t="shared" si="1"/>
         <v>1.2502166558823529</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="12">
         <v>1.5200800000000001</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="7">
+      <c r="I7" s="5">
+        <v>500</v>
+      </c>
+      <c r="J7" s="21"/>
+      <c r="K7" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L7" s="12"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="27"/>
-      <c r="O7" s="7">
+      <c r="L7" s="10">
+        <v>52.574300000000001</v>
+      </c>
+      <c r="M7" s="5"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P7" s="12"/>
+      <c r="P7" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>9</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="19">
         <v>12096142</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <f t="shared" si="0"/>
         <v>5.9294813725490197E-3</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="10">
         <v>7.9947000000000004E-3</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>15000</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="19">
         <v>5738166078</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <f t="shared" si="1"/>
         <v>2.8128265088235294</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="12">
         <v>3.2799900000000002</v>
       </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="7">
+      <c r="I8" s="5">
+        <v>600</v>
+      </c>
+      <c r="J8" s="21"/>
+      <c r="K8" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L8" s="12"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="7">
+      <c r="L8" s="10">
+        <v>118.78400000000001</v>
+      </c>
+      <c r="M8" s="5"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P8" s="12"/>
+      <c r="P8" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>10</v>
       </c>
-      <c r="B9" s="25">
+      <c r="B9" s="19">
         <v>127733917</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <f t="shared" si="0"/>
         <v>6.2614665196078431E-2</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="10">
         <v>7.2628100000000001E-2</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>20000</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="19">
         <v>10200885028</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <f t="shared" si="1"/>
         <v>5.000433837254902</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="12">
         <v>5.81569</v>
       </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="7">
+      <c r="I9" s="5">
+        <v>700</v>
+      </c>
+      <c r="J9" s="21"/>
+      <c r="K9" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L9" s="12"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="7">
+      <c r="L9" s="10">
+        <v>212.196</v>
+      </c>
+      <c r="M9" s="5"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P9" s="12"/>
+      <c r="P9" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>11</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="19">
         <v>1480550572</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <f t="shared" si="0"/>
         <v>0.72576008431372552</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="10">
         <v>0.80502700000000005</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>30000</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="19">
         <v>22951327338</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <f t="shared" si="1"/>
         <v>11.250650655882353</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="12">
         <v>13.0891</v>
       </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="7">
+      <c r="I10" s="5">
+        <v>800</v>
+      </c>
+      <c r="J10" s="21"/>
+      <c r="K10" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L10" s="12"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="27"/>
-      <c r="O10" s="7">
+      <c r="L10" s="10">
+        <v>384.61799999999999</v>
+      </c>
+      <c r="M10" s="5"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P10" s="12"/>
+      <c r="P10" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="5">
         <v>12</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11" s="19">
         <v>18681062587</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <f t="shared" si="0"/>
         <v>9.1573836210784307</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="10">
         <v>9.2938700000000001</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>50000</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11" s="19">
         <v>63752209738</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <f t="shared" si="1"/>
         <v>31.25108320490196</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="12">
         <v>36.258200000000002</v>
       </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="7">
+      <c r="I11" s="5">
+        <v>900</v>
+      </c>
+      <c r="J11" s="21"/>
+      <c r="K11" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L11" s="12"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="7">
+      <c r="L11" s="10">
+        <v>732.68100000000004</v>
+      </c>
+      <c r="M11" s="5"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P11" s="12"/>
+      <c r="P11" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="19">
+      <c r="A12" s="16">
         <v>13</v>
       </c>
-      <c r="B12" s="26">
+      <c r="B12" s="20">
         <v>248828851402</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <f>B12/$R$2</f>
         <v>121.97492715784314</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="11">
         <v>115.34099999999999</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="16">
         <v>100000</v>
       </c>
-      <c r="F12" s="20">
+      <c r="F12" s="17">
         <v>275004424058</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <f t="shared" si="1"/>
         <v>134.8060902245098</v>
       </c>
-      <c r="H12" s="17">
+      <c r="H12" s="14">
         <v>145.41999999999999</v>
       </c>
-      <c r="I12" s="19"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="8">
+      <c r="I12" s="16">
+        <v>1000</v>
+      </c>
+      <c r="J12" s="17"/>
+      <c r="K12" s="7">
         <f>J12/$R$2</f>
         <v>0</v>
       </c>
-      <c r="L12" s="13"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="8">
+      <c r="L12" s="11">
+        <v>1455.61</v>
+      </c>
+      <c r="M12" s="16"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="7">
         <f>N12/$R$2</f>
         <v>0</v>
       </c>
-      <c r="P12" s="13"/>
+      <c r="P12" s="11">
+        <f>O12/$R$2</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
remove local search algo
</commit_message>
<xml_diff>
--- a/lab4/lab4.xlsx
+++ b/lab4/lab4.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE1DCE9-F307-4D28-97E4-398180696B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635C16F9-6E9E-40D1-9095-B4E35410D7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>Значение
 счётчика</t>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>Метод ветвей и границ</t>
-  </si>
-  <si>
-    <t>Локальный поиск с выбором</t>
   </si>
   <si>
     <t>Параметры:
@@ -88,7 +85,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -176,19 +173,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -208,8 +192,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -226,7 +208,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -235,9 +216,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -248,6 +226,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1472,417 +1454,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-5141-4D2A-B2CE-37E0EC5024DC}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="193206200"/>
-        <c:axId val="193201936"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="193206200"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="193201936"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="193201936"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="193206200"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="ru-RU"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="ru-RU"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="ru-RU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Commisvoyageur Algorithms'!$O$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Время
-аналитическое</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Commisvoyageur Algorithms'!$M$3:$M$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Commisvoyageur Algorithms'!$O$3:$O$12</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4E8B-4B85-90A5-C6DCEFC30CA0}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Commisvoyageur Algorithms'!$P$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Время
-фактическое</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Commisvoyageur Algorithms'!$M$3:$M$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Commisvoyageur Algorithms'!$P$3:$P$12</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-4E8B-4B85-90A5-C6DCEFC30CA0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2209,46 +1780,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -3256,509 +2787,6 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4366,44 +3394,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>185739</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Диаграмма 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1345803-DEF2-4F3A-8B1A-8E347D197B3A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4735,9 +3725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4753,10 +3741,10 @@
     <col min="10" max="10" width="15.42578125" customWidth="1"/>
     <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.85546875" customWidth="1"/>
     <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" customWidth="1"/>
     <col min="18" max="18" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4764,603 +3752,530 @@
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="27"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="23"/>
       <c r="E1" s="4"/>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="27"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="23"/>
       <c r="I1" s="4"/>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="26"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="O1" s="26"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="23"/>
+      <c r="M1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
       <c r="P1" s="27"/>
-      <c r="R1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
-        <v>9</v>
+      <c r="A2" s="19" t="s">
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="20" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="22" t="s">
-        <v>10</v>
+      <c r="E2" s="19" t="s">
+        <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="20" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="22" t="s">
-        <v>10</v>
+      <c r="I2" s="19" t="s">
+        <v>9</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="20" t="s">
         <v>1</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R2" s="1">
+      <c r="M2" s="1">
         <v>2040000000</v>
       </c>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>4</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="16">
         <v>667</v>
       </c>
       <c r="C3" s="6">
-        <f t="shared" ref="C3:C11" si="0">B3/$R$2</f>
+        <f>B3/$M$2</f>
         <v>3.2696078431372549E-7</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="8">
         <v>0</v>
       </c>
       <c r="E3" s="5">
         <v>1000</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="16">
         <v>25543038</v>
       </c>
       <c r="G3" s="6">
-        <f t="shared" ref="G3:G12" si="1">F3/$R$2</f>
+        <f>F3/$M$2</f>
         <v>1.252109705882353E-2</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="10">
         <v>1.9010099999999999E-2</v>
       </c>
       <c r="I3" s="5">
         <v>100</v>
       </c>
-      <c r="J3" s="19">
+      <c r="J3" s="16">
         <v>158877657</v>
       </c>
       <c r="K3" s="6">
-        <f t="shared" ref="K3:K11" si="2">J3/$R$2</f>
+        <f>J3/$M$2</f>
         <v>7.7881204411764701E-2</v>
       </c>
-      <c r="L3" s="10">
+      <c r="L3" s="8">
         <v>6.70959E-2</v>
       </c>
-      <c r="M3" s="5"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="8">
-        <f t="shared" ref="O3:P11" si="3">N3/$R$2</f>
-        <v>0</v>
-      </c>
-      <c r="P3" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="R3" s="15"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="R3" s="13"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>5</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="16">
         <v>3250</v>
       </c>
       <c r="C4" s="6">
-        <f t="shared" si="0"/>
+        <f>B4/$M$2</f>
         <v>1.5931372549019608E-6</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="8">
         <v>0</v>
       </c>
       <c r="E4" s="5">
         <v>2000</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="16">
         <v>102087548</v>
       </c>
       <c r="G4" s="6">
-        <f t="shared" si="1"/>
+        <f>F4/$M$2</f>
         <v>5.004291568627451E-2</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="10">
         <v>5.5119399999999999E-2</v>
       </c>
       <c r="I4" s="5">
         <v>200</v>
       </c>
-      <c r="J4" s="19">
+      <c r="J4" s="16">
         <v>2446274152</v>
       </c>
       <c r="K4" s="6">
-        <f t="shared" si="2"/>
+        <f>J4/$M$2</f>
         <v>1.1991539960784314</v>
       </c>
-      <c r="L4" s="10">
+      <c r="L4" s="8">
         <v>0.84196899999999997</v>
       </c>
-      <c r="M4" s="5"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P4" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="M4" s="24"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>6</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="16">
         <v>20257</v>
       </c>
       <c r="C5" s="6">
-        <f t="shared" si="0"/>
+        <f>B5/$M$2</f>
         <v>9.9299019607843143E-6</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="8">
         <v>0</v>
       </c>
       <c r="E5" s="5">
         <v>3000</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="16">
         <v>229631988</v>
       </c>
       <c r="G5" s="6">
-        <f t="shared" si="1"/>
+        <f>F5/$M$2</f>
         <v>0.1125647</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="10">
         <v>0.140627</v>
       </c>
       <c r="I5" s="5">
         <v>300</v>
       </c>
-      <c r="J5" s="19">
+      <c r="J5" s="16">
         <v>12282648311</v>
       </c>
       <c r="K5" s="6">
-        <f t="shared" si="2"/>
+        <f>J5/$M$2</f>
         <v>6.0209060348039216</v>
       </c>
-      <c r="L5" s="10">
+      <c r="L5" s="8">
         <v>4.5361799999999999</v>
       </c>
-      <c r="M5" s="5"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P5" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="M5" s="24"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>7</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="16">
         <v>149872</v>
       </c>
       <c r="C6" s="6">
-        <f t="shared" si="0"/>
+        <f>B6/$M$2</f>
         <v>7.3466666666666673E-5</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="8">
         <v>0</v>
       </c>
       <c r="E6" s="5">
         <v>5000</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="16">
         <v>637721678</v>
       </c>
       <c r="G6" s="6">
-        <f t="shared" si="1"/>
+        <f>F6/$M$2</f>
         <v>0.31260866568627449</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="10">
         <v>0.41103499999999998</v>
       </c>
       <c r="I6" s="5">
         <v>400</v>
       </c>
-      <c r="J6" s="21">
+      <c r="J6" s="18">
         <v>30677967766</v>
       </c>
       <c r="K6" s="6">
-        <f t="shared" si="2"/>
+        <f>J6/$M$2</f>
         <v>15.038219493137255</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="8">
         <v>14.290699999999999</v>
       </c>
-      <c r="M6" s="5"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P6" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="M6" s="24"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>8</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="16">
         <v>1270207</v>
       </c>
       <c r="C7" s="6">
-        <f t="shared" si="0"/>
+        <f>B7/$M$2</f>
         <v>6.2265049019607848E-4</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="8">
         <v>1.0212999999999999E-3</v>
       </c>
       <c r="E7" s="5">
         <v>10000</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="16">
         <v>2550441978</v>
       </c>
       <c r="G7" s="6">
-        <f t="shared" si="1"/>
+        <f>F7/$M$2</f>
         <v>1.2502166558823529</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="10">
         <v>1.5200800000000001</v>
       </c>
       <c r="I7" s="5">
         <v>500</v>
       </c>
-      <c r="J7" s="21">
+      <c r="J7" s="18">
         <v>81257395986</v>
       </c>
       <c r="K7" s="6">
-        <f t="shared" si="2"/>
+        <f>J7/$M$2</f>
         <v>39.83205685588235</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7" s="8">
         <v>36.9831</v>
       </c>
-      <c r="M7" s="5"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P7" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="M7" s="24"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>9</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="16">
         <v>12096142</v>
       </c>
       <c r="C8" s="6">
-        <f t="shared" si="0"/>
+        <f>B8/$M$2</f>
         <v>5.9294813725490197E-3</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="8">
         <v>7.9947000000000004E-3</v>
       </c>
       <c r="E8" s="5">
         <v>15000</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="16">
         <v>5738166078</v>
       </c>
       <c r="G8" s="6">
-        <f t="shared" si="1"/>
+        <f>F8/$M$2</f>
         <v>2.8128265088235294</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="10">
         <v>3.2799900000000002</v>
       </c>
       <c r="I8" s="5">
         <v>600</v>
       </c>
-      <c r="J8" s="21">
+      <c r="J8" s="18">
         <v>195188662219</v>
       </c>
       <c r="K8" s="6">
-        <f t="shared" si="2"/>
+        <f>J8/$M$2</f>
         <v>95.680716774019615</v>
       </c>
-      <c r="L8" s="10">
+      <c r="L8" s="8">
         <v>86.5929</v>
       </c>
-      <c r="M8" s="5"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P8" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="M8" s="24"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>10</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="16">
         <v>127733917</v>
       </c>
       <c r="C9" s="6">
-        <f t="shared" si="0"/>
+        <f>B9/$M$2</f>
         <v>6.2614665196078431E-2</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="8">
         <v>7.2628100000000001E-2</v>
       </c>
       <c r="E9" s="5">
         <v>20000</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="16">
         <v>10200885028</v>
       </c>
       <c r="G9" s="6">
-        <f t="shared" si="1"/>
+        <f>F9/$M$2</f>
         <v>5.000433837254902</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="10">
         <v>5.81569</v>
       </c>
       <c r="I9" s="5">
         <v>700</v>
       </c>
-      <c r="J9" s="21">
+      <c r="J9" s="18">
         <v>331279683418</v>
       </c>
       <c r="K9" s="6">
-        <f t="shared" si="2"/>
+        <f>J9/$M$2</f>
         <v>162.39200167549021</v>
       </c>
-      <c r="L9" s="10">
+      <c r="L9" s="8">
         <v>165.357</v>
       </c>
-      <c r="M9" s="5"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P9" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="M9" s="24"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>11</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="16">
         <v>1480550572</v>
       </c>
       <c r="C10" s="6">
-        <f t="shared" si="0"/>
+        <f>B10/$M$2</f>
         <v>0.72576008431372552</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="8">
         <v>0.80502700000000005</v>
       </c>
       <c r="E10" s="5">
         <v>30000</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="16">
         <v>22951327338</v>
       </c>
       <c r="G10" s="6">
-        <f t="shared" si="1"/>
+        <f>F10/$M$2</f>
         <v>11.250650655882353</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="10">
         <v>13.0891</v>
       </c>
       <c r="I10" s="5">
         <v>800</v>
       </c>
-      <c r="J10" s="21">
+      <c r="J10" s="18">
         <v>656001849263</v>
       </c>
       <c r="K10" s="6">
-        <f t="shared" si="2"/>
+        <f>J10/$M$2</f>
         <v>321.56953395245097</v>
       </c>
-      <c r="L10" s="10">
+      <c r="L10" s="8">
         <v>328.709</v>
       </c>
-      <c r="M10" s="5"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P10" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="M10" s="24"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>12</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="16">
         <v>18681062587</v>
       </c>
       <c r="C11" s="6">
-        <f t="shared" si="0"/>
+        <f>B11/$M$2</f>
         <v>9.1573836210784307</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="8">
         <v>9.2938700000000001</v>
       </c>
       <c r="E11" s="5">
         <v>50000</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="16">
         <v>63752209738</v>
       </c>
       <c r="G11" s="6">
-        <f t="shared" si="1"/>
+        <f>F11/$M$2</f>
         <v>31.25108320490196</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="10">
         <v>36.258200000000002</v>
       </c>
       <c r="I11" s="5">
         <v>900</v>
       </c>
-      <c r="J11" s="21">
+      <c r="J11" s="18">
         <v>996322306867</v>
       </c>
       <c r="K11" s="6">
-        <f t="shared" si="2"/>
+        <f>J11/$M$2</f>
         <v>488.39328767990196</v>
       </c>
-      <c r="L11" s="10">
+      <c r="L11" s="8">
         <v>498.74400000000003</v>
       </c>
-      <c r="M11" s="5"/>
-      <c r="N11" s="21"/>
-      <c r="O11" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P11" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="M11" s="24"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
+      <c r="A12" s="14">
         <v>13</v>
       </c>
-      <c r="B12" s="20">
+      <c r="B12" s="17">
         <v>248828851402</v>
       </c>
       <c r="C12" s="7">
-        <f>B12/$R$2</f>
+        <f>B12/$M$2</f>
         <v>121.97492715784314</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="9">
         <v>115.34099999999999</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="14">
         <v>100000</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="15">
         <v>275004424058</v>
       </c>
       <c r="G12" s="7">
-        <f t="shared" si="1"/>
+        <f>F12/$M$2</f>
         <v>134.8060902245098</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="12">
         <v>145.41999999999999</v>
       </c>
-      <c r="I12" s="16">
+      <c r="I12" s="14">
         <v>1000</v>
       </c>
-      <c r="J12" s="17">
+      <c r="J12" s="15">
         <v>2102932932745</v>
       </c>
       <c r="K12" s="7">
-        <f>J12/$R$2</f>
+        <f>J12/$M$2</f>
         <v>1030.8494768357843</v>
       </c>
-      <c r="L12" s="11">
+      <c r="L12" s="9">
         <v>941.93700000000001</v>
       </c>
-      <c r="M12" s="16"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="7">
-        <f>N12/$R$2</f>
-        <v>0</v>
-      </c>
-      <c r="P12" s="11">
-        <f>O12/$R$2</f>
-        <v>0</v>
-      </c>
+      <c r="M12" s="24"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="J1:L1"/>
-    <mergeCell ref="N1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>